<commit_message>
Added Updated Product backlog
1) Added updated product backlog for sprint 3
</commit_message>
<xml_diff>
--- a/sprints/Product Backlog.xlsx
+++ b/sprints/Product Backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swamp\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swamp\Desktop\CapstoneGroup3\sprints\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B5FCEAE-2103-4530-AF0C-2373C327AB6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4394AF12-10D4-4FCD-A364-81C48C89F44A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -92,9 +92,6 @@
     <t>I can assign a name and description for the project to help others understand the purpose of the project</t>
   </si>
   <si>
-    <t>View and Edit a Board for a Project</t>
-  </si>
-  <si>
     <t>I can define the Stages of work expected for a project and setup for any handoffs needed during project work</t>
   </si>
   <si>
@@ -119,9 +116,6 @@
     <t>I can define work needed for a Project for my Group</t>
   </si>
   <si>
-    <t>Update Status of my assigned Task</t>
-  </si>
-  <si>
     <t>I can notify others about the progress on a Task</t>
   </si>
   <si>
@@ -171,6 +165,12 @@
   </si>
   <si>
     <t>All features available to Employees are also available to Managers and Admins</t>
+  </si>
+  <si>
+    <t>Edit a Board for a Project</t>
+  </si>
+  <si>
+    <t>Update Stage of my assigned Task</t>
   </si>
 </sst>
 </file>
@@ -186,7 +186,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -205,6 +205,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -218,7 +224,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -231,6 +237,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -515,19 +524,19 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="16.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="48.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="74.85546875" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.1796875" style="2"/>
+    <col min="2" max="2" width="16.7265625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="48.54296875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="74.81640625" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="9.1796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -541,189 +550,189 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="5">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
+    <row r="3" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="5">
+        <v>0</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>1</v>
-      </c>
-      <c r="B4" s="3" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="5">
+        <v>0</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="5">
+        <v>0</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D6" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>1</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="3" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D7" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>1</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>1</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>1</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>1</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D9" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="3">
+        <v>1</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <v>2</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="C10" s="3" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>2</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>3</v>
       </c>
@@ -731,74 +740,74 @@
         <v>11</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
+        <v>3</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" s="3">
+        <v>3</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A18" s="3">
         <v>4</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="3" t="s">
+      <c r="B18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D18" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
-        <v>4</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
-        <v>5</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="3" t="s">
+    <row r="19" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="B19" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="C19" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B19" s="4" t="s">
+    <row r="20" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="B20" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B20" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D18">
-    <sortCondition ref="A2:A18"/>
-    <sortCondition ref="B2:B18"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D20">
+    <sortCondition ref="A2:A20"/>
+    <sortCondition ref="B2:B20"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>